<commit_message>
Update Data Collection Notes.xlsx
</commit_message>
<xml_diff>
--- a/DataCollection/Data Collection Notes.xlsx
+++ b/DataCollection/Data Collection Notes.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Intel\Documents\GitHub\Muscle_Sensory\DataCollection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF5C8DE3-EA6D-4B99-95C5-A8FBE9789552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A09CFBA1-62C2-46F5-9CFE-B42A26CAC97C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Dec8 - 10mm Unkinked" sheetId="1" r:id="rId1"/>
+    <sheet name="Dec16-10mmKinked" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -492,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G40" sqref="A14:G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,74 +744,290 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C7DEB1B-4EB0-4CB2-80F8-B0D1F00A8160}">
+  <dimension ref="A1:G27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5">
+        <v>10</v>
+      </c>
+      <c r="D4" s="5">
+        <v>500</v>
+      </c>
+      <c r="E4" s="5">
+        <v>30</v>
+      </c>
+      <c r="F4" s="5">
+        <v>500</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" s="5">
+        <v>10</v>
+      </c>
+      <c r="D5" s="5">
+        <v>500</v>
+      </c>
+      <c r="E5" s="5">
+        <v>30</v>
+      </c>
+      <c r="F5" s="5">
+        <v>500</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" s="5">
+        <v>10</v>
+      </c>
+      <c r="D6" s="5">
+        <v>500</v>
+      </c>
+      <c r="E6" s="5">
+        <v>40</v>
+      </c>
+      <c r="F6" s="5">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7" s="5">
+        <v>10</v>
+      </c>
+      <c r="D7" s="5">
+        <v>500</v>
+      </c>
+      <c r="E7" s="5">
+        <v>40</v>
+      </c>
+      <c r="F7" s="5">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8" s="5">
+        <v>10</v>
+      </c>
+      <c r="D8" s="5">
+        <v>500</v>
+      </c>
+      <c r="E8" s="5">
+        <v>60</v>
+      </c>
+      <c r="F8" s="5">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9" s="5">
+        <v>10</v>
+      </c>
+      <c r="D9" s="5">
+        <v>500</v>
+      </c>
+      <c r="E9" s="5">
+        <v>60</v>
+      </c>
+      <c r="F9" s="5">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>7</v>
+      </c>
+      <c r="C10" s="5">
+        <v>5</v>
+      </c>
+      <c r="D10" s="5">
+        <v>500</v>
+      </c>
+      <c r="E10" s="5">
+        <v>40</v>
+      </c>
+      <c r="F10" s="5">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11" s="5">
+        <v>5</v>
+      </c>
+      <c r="D11" s="5">
+        <v>500</v>
+      </c>
+      <c r="E11" s="5">
+        <v>40</v>
+      </c>
+      <c r="F11" s="5">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>9</v>
+      </c>
+      <c r="C12" s="5">
+        <v>5</v>
+      </c>
+      <c r="D12" s="5">
+        <v>500</v>
+      </c>
+      <c r="E12" s="5">
+        <v>50</v>
+      </c>
+      <c r="F12" s="5">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13" s="8">
+        <v>5</v>
+      </c>
+      <c r="D13" s="8">
+        <v>500</v>
+      </c>
+      <c r="E13" s="8">
+        <v>50</v>
+      </c>
+      <c r="F13" s="8">
+        <v>500</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>7</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>12</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>13</v>
       </c>
-      <c r="F15" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="F16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B17" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C17" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16" s="5" t="s">
+      <c r="D17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F17" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17" s="5">
-        <v>10</v>
-      </c>
-      <c r="D17" s="5">
-        <v>500</v>
-      </c>
-      <c r="E17" s="5">
-        <v>30</v>
-      </c>
-      <c r="F17" s="5">
-        <v>500</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>16</v>
+      <c r="G17" s="6" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18" s="5">
         <v>10</v>
@@ -824,13 +1041,11 @@
       <c r="F18" s="5">
         <v>500</v>
       </c>
-      <c r="G18" s="10" t="s">
-        <v>17</v>
-      </c>
+      <c r="G18" s="10"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C19" s="5">
         <v>10</v>
@@ -839,15 +1054,16 @@
         <v>500</v>
       </c>
       <c r="E19" s="5">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="F19" s="5">
         <v>500</v>
       </c>
+      <c r="G19" s="10"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C20" s="5">
         <v>10</v>
@@ -864,7 +1080,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C21" s="5">
         <v>10</v>
@@ -873,7 +1089,7 @@
         <v>500</v>
       </c>
       <c r="E21" s="5">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="F21" s="5">
         <v>500</v>
@@ -881,7 +1097,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C22" s="5">
         <v>10</v>
@@ -898,16 +1114,16 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C23" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D23" s="5">
         <v>500</v>
       </c>
       <c r="E23" s="5">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="F23" s="5">
         <v>500</v>
@@ -915,7 +1131,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B24">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C24" s="5">
         <v>5</v>
@@ -932,252 +1148,52 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B25">
+        <v>8</v>
+      </c>
+      <c r="C25" s="5">
+        <v>5</v>
+      </c>
+      <c r="D25" s="5">
+        <v>500</v>
+      </c>
+      <c r="E25" s="5">
+        <v>40</v>
+      </c>
+      <c r="F25" s="5">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26">
         <v>9</v>
       </c>
-      <c r="C25" s="5">
-        <v>5</v>
-      </c>
-      <c r="D25" s="5">
-        <v>500</v>
-      </c>
-      <c r="E25" s="5">
+      <c r="C26" s="5">
+        <v>5</v>
+      </c>
+      <c r="D26" s="5">
+        <v>500</v>
+      </c>
+      <c r="E26" s="5">
         <v>50</v>
       </c>
-      <c r="F25" s="5">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26">
-        <v>10</v>
-      </c>
-      <c r="C26" s="8">
-        <v>5</v>
-      </c>
-      <c r="D26" s="8">
-        <v>500</v>
-      </c>
-      <c r="E26" s="8">
+      <c r="F26" s="5">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <v>10</v>
+      </c>
+      <c r="C27" s="8">
+        <v>5</v>
+      </c>
+      <c r="D27" s="8">
+        <v>500</v>
+      </c>
+      <c r="E27" s="8">
         <v>50</v>
       </c>
-      <c r="F26" s="8">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" t="s">
-        <v>12</v>
-      </c>
-      <c r="D29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F29" t="s">
-        <v>18</v>
-      </c>
-      <c r="G29" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G30" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31" s="5">
-        <v>10</v>
-      </c>
-      <c r="D31" s="5">
-        <v>500</v>
-      </c>
-      <c r="E31" s="5">
-        <v>30</v>
-      </c>
-      <c r="F31" s="5">
-        <v>500</v>
-      </c>
-      <c r="G31" s="10"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B32">
-        <v>2</v>
-      </c>
-      <c r="C32" s="5">
-        <v>10</v>
-      </c>
-      <c r="D32" s="5">
-        <v>500</v>
-      </c>
-      <c r="E32" s="5">
-        <v>30</v>
-      </c>
-      <c r="F32" s="5">
-        <v>500</v>
-      </c>
-      <c r="G32" s="10"/>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33">
-        <v>3</v>
-      </c>
-      <c r="C33" s="5">
-        <v>10</v>
-      </c>
-      <c r="D33" s="5">
-        <v>500</v>
-      </c>
-      <c r="E33" s="5">
-        <v>40</v>
-      </c>
-      <c r="F33" s="5">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34">
-        <v>4</v>
-      </c>
-      <c r="C34" s="5">
-        <v>10</v>
-      </c>
-      <c r="D34" s="5">
-        <v>500</v>
-      </c>
-      <c r="E34" s="5">
-        <v>40</v>
-      </c>
-      <c r="F34" s="5">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35">
-        <v>5</v>
-      </c>
-      <c r="C35" s="5">
-        <v>10</v>
-      </c>
-      <c r="D35" s="5">
-        <v>500</v>
-      </c>
-      <c r="E35" s="5">
-        <v>60</v>
-      </c>
-      <c r="F35" s="5">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36">
-        <v>6</v>
-      </c>
-      <c r="C36" s="5">
-        <v>10</v>
-      </c>
-      <c r="D36" s="5">
-        <v>500</v>
-      </c>
-      <c r="E36" s="5">
-        <v>60</v>
-      </c>
-      <c r="F36" s="5">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37">
-        <v>7</v>
-      </c>
-      <c r="C37" s="5">
-        <v>5</v>
-      </c>
-      <c r="D37" s="5">
-        <v>500</v>
-      </c>
-      <c r="E37" s="5">
-        <v>40</v>
-      </c>
-      <c r="F37" s="5">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38">
-        <v>8</v>
-      </c>
-      <c r="C38" s="5">
-        <v>5</v>
-      </c>
-      <c r="D38" s="5">
-        <v>500</v>
-      </c>
-      <c r="E38" s="5">
-        <v>40</v>
-      </c>
-      <c r="F38" s="5">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B39">
-        <v>9</v>
-      </c>
-      <c r="C39" s="5">
-        <v>5</v>
-      </c>
-      <c r="D39" s="5">
-        <v>500</v>
-      </c>
-      <c r="E39" s="5">
-        <v>50</v>
-      </c>
-      <c r="F39" s="5">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40">
-        <v>10</v>
-      </c>
-      <c r="C40" s="8">
-        <v>5</v>
-      </c>
-      <c r="D40" s="8">
-        <v>500</v>
-      </c>
-      <c r="E40" s="8">
-        <v>50</v>
-      </c>
-      <c r="F40" s="8">
+      <c r="F27" s="8">
         <v>500</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New 8mm Kinked Data
</commit_message>
<xml_diff>
--- a/DataCollection/Data Collection Notes.xlsx
+++ b/DataCollection/Data Collection Notes.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Intel\Documents\GitHub\Muscle_Sensory\DataCollection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A09CFBA1-62C2-46F5-9CFE-B42A26CAC97C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{790D6A4B-9DD3-45B0-B29F-947CA6FC0F3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24390" yWindow="2010" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dec8 - 10mm Unkinked" sheetId="1" r:id="rId1"/>
     <sheet name="Dec16-10mmKinked" sheetId="2" r:id="rId2"/>
+    <sheet name="Dec21-8mmkink" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
   <si>
     <t>10mm BPA Data Collection</t>
   </si>
@@ -86,6 +87,9 @@
   </si>
   <si>
     <t>End to end length =0.4-0.5</t>
+  </si>
+  <si>
+    <t>8mm kinked</t>
   </si>
 </sst>
 </file>
@@ -753,7 +757,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C7DEB1B-4EB0-4CB2-80F8-B0D1F00A8160}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
@@ -1200,4 +1204,24 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E11394F-5D41-4215-A116-20E3A1062556}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
correcting 10mm and 20mm data
</commit_message>
<xml_diff>
--- a/DataCollection/Data Collection Notes.xlsx
+++ b/DataCollection/Data Collection Notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lawre\Documents\GitHub\Muscle-Sensory\DataCollection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB602D44-E200-4C57-9BCD-F03F1B1685E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B0D77F8-87D1-45FD-8C3B-CE51EA0718E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-13068" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dec8 - 10mm13cm" sheetId="1" r:id="rId1"/>
@@ -571,10 +571,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1544,7 +1540,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="I8" sqref="A1:J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2027,7 +2023,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>